<commit_message>
Added another test photo club (FC dG)
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/LineCount.xlsx
+++ b/Fotogroep Waalre/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC90D6B-E4CD-9946-8427-078A573A9A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61489BE1-B871-FA44-A883-A0C74AF3B2C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1362,7 +1362,7 @@
                   <c:v>5241</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>5279</c:v>
+                  <c:v>5404</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2509,7 +2509,7 @@
                   <c:v>4158</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>4180</c:v>
+                  <c:v>4278</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3658,7 +3658,7 @@
                   <c:v>598</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>610</c:v>
+                  <c:v>624</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4826,7 +4826,7 @@
                   <c:v>485</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>489</c:v>
+                  <c:v>502</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4919,7 +4919,7 @@
         <c:axId val="1582338719"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="5500"/>
+          <c:max val="6000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -12877,20 +12877,20 @@
         <v>197</v>
       </c>
       <c r="G184" s="4">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H184">
         <f t="shared" si="283"/>
-        <v>5279</v>
+        <v>5404</v>
       </c>
       <c r="I184" s="5">
-        <v>4180</v>
+        <v>4278</v>
       </c>
       <c r="J184" s="6">
-        <v>610</v>
+        <v>624</v>
       </c>
       <c r="K184" s="7">
-        <v>489</v>
+        <v>502</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more members for Fotogroep Anders.
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/LineCount.xlsx
+++ b/Fotogroep Waalre/Documentation/LineCount.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A12503-F9F3-4F4C-AEEF-FC773D22CF9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477E0B63-A9B1-4D45-AB2C-4D768F982238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -824,6 +824,9 @@
                 <c:pt idx="186">
                   <c:v>45222</c:v>
                 </c:pt>
+                <c:pt idx="187">
+                  <c:v>45231</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1393,6 +1396,9 @@
                 </c:pt>
                 <c:pt idx="186">
                   <c:v>5544</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>5705</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2001,6 +2007,9 @@
                 <c:pt idx="186">
                   <c:v>45222</c:v>
                 </c:pt>
+                <c:pt idx="187">
+                  <c:v>45231</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2570,6 +2579,9 @@
                 </c:pt>
                 <c:pt idx="186">
                   <c:v>4343</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>4481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3180,6 +3192,9 @@
                 <c:pt idx="186">
                   <c:v>45222</c:v>
                 </c:pt>
+                <c:pt idx="187">
+                  <c:v>45231</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3749,6 +3764,9 @@
                 </c:pt>
                 <c:pt idx="186">
                   <c:v>672</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>686</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4378,6 +4396,9 @@
                 <c:pt idx="186">
                   <c:v>45222</c:v>
                 </c:pt>
+                <c:pt idx="187">
+                  <c:v>45231</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4947,6 +4968,9 @@
                 </c:pt>
                 <c:pt idx="186">
                   <c:v>529</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>538</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4973,7 +4997,7 @@
         <c:axId val="1582352671"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="45230"/>
+          <c:max val="45260"/>
           <c:min val="44379"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -6175,13 +6199,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K189"/>
+  <dimension ref="A1:K190"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B167" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A190" sqref="A190"/>
+      <selection pane="bottomRight" activeCell="G191" sqref="G191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13196,6 +13220,43 @@
       </c>
       <c r="K189" s="7">
         <v>529</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A190" s="1">
+        <v>45231</v>
+      </c>
+      <c r="B190" s="2">
+        <v>9</v>
+      </c>
+      <c r="C190">
+        <f t="shared" ref="C190" si="295">SUM(D190:F190)</f>
+        <v>1673</v>
+      </c>
+      <c r="D190">
+        <v>1105</v>
+      </c>
+      <c r="E190">
+        <v>371</v>
+      </c>
+      <c r="F190" s="3">
+        <v>197</v>
+      </c>
+      <c r="G190" s="4">
+        <v>68</v>
+      </c>
+      <c r="H190">
+        <f t="shared" ref="H190" si="296">SUM(I190:K190)</f>
+        <v>5705</v>
+      </c>
+      <c r="I190" s="5">
+        <v>4481</v>
+      </c>
+      <c r="J190" s="6">
+        <v>686</v>
+      </c>
+      <c r="K190" s="7">
+        <v>538</v>
       </c>
     </row>
   </sheetData>
@@ -13215,7 +13276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA32" sqref="AA32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated readme file (because of Release 2.5.0) and line count stats.
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/LineCount.xlsx
+++ b/Fotogroep Waalre/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477E0B63-A9B1-4D45-AB2C-4D768F982238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9879B8-8AC3-B046-A1D3-E42CABA897E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -827,6 +827,9 @@
                 <c:pt idx="187">
                   <c:v>45231</c:v>
                 </c:pt>
+                <c:pt idx="188">
+                  <c:v>45233</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1399,6 +1402,9 @@
                 </c:pt>
                 <c:pt idx="187">
                   <c:v>5705</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>5709</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2010,6 +2016,9 @@
                 <c:pt idx="187">
                   <c:v>45231</c:v>
                 </c:pt>
+                <c:pt idx="188">
+                  <c:v>45233</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2582,6 +2591,9 @@
                 </c:pt>
                 <c:pt idx="187">
                   <c:v>4481</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>4464</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3195,6 +3207,9 @@
                 <c:pt idx="187">
                   <c:v>45231</c:v>
                 </c:pt>
+                <c:pt idx="188">
+                  <c:v>45233</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3767,6 +3782,9 @@
                 </c:pt>
                 <c:pt idx="187">
                   <c:v>686</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>695</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4399,6 +4417,9 @@
                 <c:pt idx="187">
                   <c:v>45231</c:v>
                 </c:pt>
+                <c:pt idx="188">
+                  <c:v>45233</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4971,6 +4992,9 @@
                 </c:pt>
                 <c:pt idx="187">
                   <c:v>538</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>550</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6199,13 +6223,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K190"/>
+  <dimension ref="A1:K191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B167" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G191" sqref="G191"/>
+      <selection pane="bottomRight" activeCell="A191" sqref="A191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13257,6 +13281,43 @@
       </c>
       <c r="K190" s="7">
         <v>538</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A191" s="1">
+        <v>45233</v>
+      </c>
+      <c r="B191" s="2">
+        <v>9</v>
+      </c>
+      <c r="C191">
+        <f t="shared" ref="C191" si="297">SUM(D191:F191)</f>
+        <v>1673</v>
+      </c>
+      <c r="D191">
+        <v>1105</v>
+      </c>
+      <c r="E191">
+        <v>371</v>
+      </c>
+      <c r="F191" s="3">
+        <v>197</v>
+      </c>
+      <c r="G191" s="4">
+        <v>68</v>
+      </c>
+      <c r="H191">
+        <f t="shared" ref="H191" si="298">SUM(I191:K191)</f>
+        <v>5709</v>
+      </c>
+      <c r="I191" s="5">
+        <v>4464</v>
+      </c>
+      <c r="J191" s="6">
+        <v>695</v>
+      </c>
+      <c r="K191" s="7">
+        <v>550</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Translation type in NL
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/LineCount.xlsx
+++ b/Fotogroep Waalre/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9879B8-8AC3-B046-A1D3-E42CABA897E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50814FBD-C635-E747-9693-70D90901A54F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -830,6 +830,9 @@
                 <c:pt idx="188">
                   <c:v>45233</c:v>
                 </c:pt>
+                <c:pt idx="189">
+                  <c:v>45240</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1405,6 +1408,9 @@
                 </c:pt>
                 <c:pt idx="188">
                   <c:v>5709</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>5724</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2019,6 +2025,9 @@
                 <c:pt idx="188">
                   <c:v>45233</c:v>
                 </c:pt>
+                <c:pt idx="189">
+                  <c:v>45240</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2594,6 +2603,9 @@
                 </c:pt>
                 <c:pt idx="188">
                   <c:v>4464</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>4470</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3210,6 +3222,9 @@
                 <c:pt idx="188">
                   <c:v>45233</c:v>
                 </c:pt>
+                <c:pt idx="189">
+                  <c:v>45240</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3785,6 +3800,9 @@
                 </c:pt>
                 <c:pt idx="188">
                   <c:v>695</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>700</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4420,6 +4438,9 @@
                 <c:pt idx="188">
                   <c:v>45233</c:v>
                 </c:pt>
+                <c:pt idx="189">
+                  <c:v>45240</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4995,6 +5016,9 @@
                 </c:pt>
                 <c:pt idx="188">
                   <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>554</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6223,13 +6247,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K191"/>
+  <dimension ref="A1:K192"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B167" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A191" sqref="A191"/>
+      <selection pane="bottomRight" activeCell="I193" sqref="I193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13318,6 +13342,43 @@
       </c>
       <c r="K191" s="7">
         <v>550</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A192" s="1">
+        <v>45240</v>
+      </c>
+      <c r="B192" s="2">
+        <v>9</v>
+      </c>
+      <c r="C192">
+        <f t="shared" ref="C192" si="299">SUM(D192:F192)</f>
+        <v>1673</v>
+      </c>
+      <c r="D192">
+        <v>1105</v>
+      </c>
+      <c r="E192">
+        <v>371</v>
+      </c>
+      <c r="F192" s="3">
+        <v>197</v>
+      </c>
+      <c r="G192" s="4">
+        <v>68</v>
+      </c>
+      <c r="H192">
+        <f t="shared" ref="H192" si="300">SUM(I192:K192)</f>
+        <v>5724</v>
+      </c>
+      <c r="I192" s="5">
+        <v>4470</v>
+      </c>
+      <c r="J192" s="6">
+        <v>700</v>
+      </c>
+      <c r="K192" s="7">
+        <v>554</v>
       </c>
     </row>
   </sheetData>
@@ -13337,7 +13398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AA32" sqref="AA32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
mapControls     - rotate     - 3D     - scale
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/LineCount.xlsx
+++ b/Fotogroep Waalre/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D934CF-3931-D540-AA28-04F5F89152D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843C970C-74B9-1D4D-9722-77D0BBB9F292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -839,6 +839,9 @@
                 <c:pt idx="191">
                   <c:v>45249</c:v>
                 </c:pt>
+                <c:pt idx="192">
+                  <c:v>45252</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1423,6 +1426,9 @@
                 </c:pt>
                 <c:pt idx="191">
                   <c:v>5857</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>5861</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2046,6 +2052,9 @@
                 <c:pt idx="191">
                   <c:v>45249</c:v>
                 </c:pt>
+                <c:pt idx="192">
+                  <c:v>45252</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2630,6 +2639,9 @@
                 </c:pt>
                 <c:pt idx="191">
                   <c:v>4600</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>4608</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3255,6 +3267,9 @@
                 <c:pt idx="191">
                   <c:v>45249</c:v>
                 </c:pt>
+                <c:pt idx="192">
+                  <c:v>45252</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3839,6 +3854,9 @@
                 </c:pt>
                 <c:pt idx="191">
                   <c:v>704</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>701</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4483,6 +4501,9 @@
                 <c:pt idx="191">
                   <c:v>45249</c:v>
                 </c:pt>
+                <c:pt idx="192">
+                  <c:v>45252</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5067,6 +5088,9 @@
                 </c:pt>
                 <c:pt idx="191">
                   <c:v>553</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>552</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6295,13 +6319,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K194"/>
+  <dimension ref="A1:K195"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B167" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I195" sqref="I195"/>
+      <selection pane="bottomRight" activeCell="I196" sqref="I196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13501,6 +13525,43 @@
       </c>
       <c r="K194" s="7">
         <v>553</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A195" s="1">
+        <v>45252</v>
+      </c>
+      <c r="B195" s="2">
+        <v>9</v>
+      </c>
+      <c r="C195">
+        <f t="shared" ref="C195" si="305">SUM(D195:F195)</f>
+        <v>1673</v>
+      </c>
+      <c r="D195">
+        <v>1105</v>
+      </c>
+      <c r="E195">
+        <v>371</v>
+      </c>
+      <c r="F195" s="3">
+        <v>197</v>
+      </c>
+      <c r="G195" s="4">
+        <v>69</v>
+      </c>
+      <c r="H195">
+        <f t="shared" ref="H195" si="306">SUM(I195:K195)</f>
+        <v>5861</v>
+      </c>
+      <c r="I195" s="5">
+        <v>4608</v>
+      </c>
+      <c r="J195" s="6">
+        <v>701</v>
+      </c>
+      <c r="K195" s="7">
+        <v>552</v>
       </c>
     </row>
   </sheetData>

</xml_diff>